<commit_message>
flow correct factura B
</commit_message>
<xml_diff>
--- a/facturador_test.xlsx
+++ b/facturador_test.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-75" yWindow="15" windowWidth="14235" windowHeight="11640" tabRatio="609" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" tabRatio="609" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="145621" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -728,24 +728,24 @@
   </sheetPr>
   <dimension ref="A1:BR108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13.8"/>
   <cols>
-    <col width="20.875" customWidth="1" style="3" min="1" max="1"/>
-    <col width="12.375" customWidth="1" style="5" min="2" max="2"/>
-    <col width="13.25" customWidth="1" style="5" min="3" max="3"/>
-    <col width="13.5" customWidth="1" style="23" min="4" max="4"/>
-    <col width="12.75" customWidth="1" style="23" min="5" max="5"/>
-    <col width="12.75" customWidth="1" style="24" min="6" max="6"/>
-    <col width="13.25" customWidth="1" style="6" min="7" max="7"/>
-    <col width="13.75" customWidth="1" style="7" min="8" max="8"/>
-    <col width="13.125" customWidth="1" style="7" min="9" max="9"/>
-    <col width="11.375" customWidth="1" style="7" min="10" max="38"/>
-    <col width="11.375" customWidth="1" style="3" min="39" max="47"/>
-    <col width="11.375" customWidth="1" style="3" min="48" max="16384"/>
+    <col width="20.88671875" customWidth="1" style="3" min="1" max="1"/>
+    <col width="12.33203125" customWidth="1" style="5" min="2" max="2"/>
+    <col width="13.21875" customWidth="1" style="5" min="3" max="3"/>
+    <col width="13.44140625" customWidth="1" style="23" min="4" max="4"/>
+    <col width="12.77734375" customWidth="1" style="23" min="5" max="5"/>
+    <col width="12.77734375" customWidth="1" style="24" min="6" max="6"/>
+    <col width="13.21875" customWidth="1" style="6" min="7" max="7"/>
+    <col width="13.77734375" customWidth="1" style="7" min="8" max="8"/>
+    <col width="13.109375" customWidth="1" style="7" min="9" max="9"/>
+    <col width="11.33203125" customWidth="1" style="7" min="10" max="38"/>
+    <col width="11.33203125" customWidth="1" style="3" min="39" max="48"/>
+    <col width="11.33203125" customWidth="1" style="3" min="49" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customFormat="1" customHeight="1" s="7">
@@ -872,7 +872,7 @@
       </c>
       <c r="H2" s="11" t="inlineStr">
         <is>
-          <t>15/11/2024</t>
+          <t>17/11/2024</t>
         </is>
       </c>
       <c r="I2" s="12" t="inlineStr">
@@ -931,7 +931,7 @@
         </is>
       </c>
       <c r="D3" s="9" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="26">
         <f>+D3*0.21</f>
@@ -946,7 +946,7 @@
       </c>
       <c r="H3" s="11" t="inlineStr">
         <is>
-          <t>15/11/2024</t>
+          <t>17/11/2024</t>
         </is>
       </c>
       <c r="I3" s="12" t="inlineStr">

</xml_diff>